<commit_message>
Update Athasian Gladiator Planning.xlsx
</commit_message>
<xml_diff>
--- a/_notes_/Athasian Gladiator Planning.xlsx
+++ b/_notes_/Athasian Gladiator Planning.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Possible Feats / Class Abilities</t>
   </si>
@@ -34,49 +34,184 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Trade Secret: Alchemy Dealer will require detecting the merchant &amp; doubling the bard's appraise skill for the transaction.</t>
-  </si>
-  <si>
-    <t>We'd need to add a check for this for every Bluff &amp; Diplomacy check.</t>
-  </si>
-  <si>
-    <t>We'd need to add a check for this for in the Poisoncrafting System.</t>
-  </si>
-  <si>
-    <t>Trade Secret: Poison Dealer will require detecting the merchant &amp; doubling the bard's appraise skill for the transaction.</t>
-  </si>
-  <si>
-    <t>Trade Secret: Poisonbane may actually be possible, I just don't know enough about crafting to be sure.</t>
-  </si>
-  <si>
-    <t>Trade Secret: Scorpion's Touch, may be possible w/ future NWN updates</t>
-  </si>
-  <si>
-    <t>Pick Pocket will be renamed Sleight of Hand</t>
-  </si>
-  <si>
-    <t>Just need a function to combine smokestick + poison to make new grenade type.  Possible but will require a lot of item creation.</t>
-  </si>
-  <si>
-    <t>It's not possible to add class skills to a PC, even w/ NWNxEE</t>
-  </si>
-  <si>
-    <t>May be possible if we set Spring Attack temporarily while applying poison to weapon</t>
-  </si>
-  <si>
-    <t>Rerolling *any* roll simply isn't possible.</t>
-  </si>
-  <si>
-    <t>It's not possible to modify initiative, even with NWNxEE.</t>
-  </si>
-  <si>
-    <t>The closest thing to this in NWN is Uncanny Dodge</t>
-  </si>
-  <si>
-    <t>Currently not possible in NWNxEE, but apparently code could be written to do this.</t>
-  </si>
-  <si>
     <t>Gladiator Level</t>
+  </si>
+  <si>
+    <t>Armor Proficency: Heavy</t>
+  </si>
+  <si>
+    <t>Armor Proficency: Light</t>
+  </si>
+  <si>
+    <t>Armor Proficency: Medium</t>
+  </si>
+  <si>
+    <t>Weapon Prof: Simple</t>
+  </si>
+  <si>
+    <t>Weapon Prof: Martial</t>
+  </si>
+  <si>
+    <t>Shield Proficiency</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Combat Stance</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Martial Display</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Team Strike</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Taunt</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Trick</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Shake Off</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Chant</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>6th</t>
+  </si>
+  <si>
+    <t>9th</t>
+  </si>
+  <si>
+    <t>12th</t>
+  </si>
+  <si>
+    <t>15th</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Threatening Glare</t>
+  </si>
+  <si>
+    <t>18th</t>
+  </si>
+  <si>
+    <t>Gladiatorial Performance: Dragon's Fury</t>
+  </si>
+  <si>
+    <t>Mercy?</t>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>Exotic Weapon Prof #1</t>
+  </si>
+  <si>
+    <t>Exotic Weapon Prof #2</t>
+  </si>
+  <si>
+    <t>Improved Unarmed Strike</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>Arena Guile</t>
+  </si>
+  <si>
+    <t>Improved Feint</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>Uncanny Dodge</t>
+  </si>
+  <si>
+    <t>Armor Optimization I</t>
+  </si>
+  <si>
+    <t>Armor Optimization III</t>
+  </si>
+  <si>
+    <t>10th</t>
+  </si>
+  <si>
+    <t>Armor Optimization II</t>
+  </si>
+  <si>
+    <t>No Mercy?</t>
+  </si>
+  <si>
+    <t>8th</t>
+  </si>
+  <si>
+    <t>Inproved Uncanny Dodge</t>
+  </si>
+  <si>
+    <t>20th</t>
+  </si>
+  <si>
+    <t>Armor Optimization IV</t>
+  </si>
+  <si>
+    <t>Armor is treated as one category lighter (e.g. medium armor is treated as light armor).</t>
+  </si>
+  <si>
+    <t>14th</t>
+  </si>
+  <si>
+    <t>Parry?</t>
+  </si>
+  <si>
+    <t>Beginning at 14th level, once per round you can forfeit an attack to attempt to parry an incoming melee attack. The forfeited attack has to be the one with your highest base attack bonus. If wielding two weapons, the parry must be made using your primary weapon. You make an opposed attack roll with a –5 penalty against your attacker roll. If you succeed, the attack is parried and you suffer no damage or ill effects related to the attack, including touch attacks used to deliver spells.</t>
+  </si>
+  <si>
+    <t>Beginning at 6th level, you can perform a coup de grace as a standard action rather than a full‐round action.</t>
+  </si>
+  <si>
+    <t>At 1st level, you suffer no penalty to attack rolls when attacking with a weapon to inflict nonlethal damage.</t>
+  </si>
+  <si>
+    <t>Exotic Weapon Prof #3</t>
+  </si>
+  <si>
+    <t>13th</t>
+  </si>
+  <si>
+    <t>Exotic Weapon Prof #4</t>
+  </si>
+  <si>
+    <t>Weapon Prof: Exotic</t>
+  </si>
+  <si>
+    <t>Armor Optimization</t>
+  </si>
+  <si>
+    <t>17th</t>
+  </si>
+  <si>
+    <t>Exotic Weapon Prof #5</t>
+  </si>
+  <si>
+    <t>Superior Feint</t>
+  </si>
+  <si>
+    <t>16th</t>
+  </si>
+  <si>
+    <t>Improved Parry?</t>
+  </si>
+  <si>
+    <t>As parry (see above), except you no longer suffer a –5 penalty to your opposed attack roll.</t>
+  </si>
+  <si>
+    <t>Improved Parry</t>
+  </si>
+  <si>
+    <t>Weapon Specialization</t>
   </si>
 </sst>
 </file>
@@ -159,9 +294,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -185,6 +317,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -481,205 +616,393 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A37" sqref="A37:A65"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41" style="2" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="116.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="116.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" s="12"/>
+      <c r="B6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" s="13"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="C8" s="6"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="8"/>
+      <c r="A17" s="6"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="8"/>
+      <c r="A19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="6"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="8"/>
-      <c r="F21" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="A21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6"/>
+      <c r="C22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="F24" s="9" t="s">
-        <v>7</v>
+      <c r="A24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="F25" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="A25" s="7"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="F26" s="9" t="s">
-        <v>9</v>
+      <c r="A26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="F27" s="9" t="s">
-        <v>10</v>
+      <c r="A27" s="7"/>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="F29" s="9" t="s">
-        <v>11</v>
+      <c r="A29" s="7"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="E36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="F37" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="F38" s="9" t="s">
-        <v>13</v>
+      <c r="A38" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="F39" s="9" t="s">
-        <v>14</v>
+      <c r="A39" s="7"/>
+      <c r="D39" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="7"/>
+      <c r="D40" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="8"/>
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="8"/>
-      <c r="F43" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="A43" s="7"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="F44" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="A44" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="7"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="8"/>
-      <c r="F46" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="7"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="8"/>
-      <c r="F48" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="8"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="8"/>
-      <c r="F52" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="8"/>
-      <c r="F54" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="8"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="8"/>
-      <c r="F58" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="8"/>
-      <c r="F60" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="8"/>
+      <c r="A48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="7"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="7"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="7"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="7"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="7"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="7"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="7"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="7"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="7"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="7"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="7"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:B7"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>